<commit_message>
Summary: First "normal" commit. Updated TC_super.m-associated scripts for basic parameter tests and nondim; mpi, Cd, and others have not yet been tested.
Details:
Updated commit, with all files in the TC_super.m superscript updated to work properly for the basic parametric sensitivity test simulation sets.  Not all of the MPI runs have had TC_stats performed yet, and thus those still need to be tested.

Created and wrote Cd_retrieve.m to grab the value for Cd from the namelist file so that the Cd scaling can be tested without any user input.

Created Ld_nocollapse_r.m to show NH/f does not work for size scaling, but haven't yet updated this at all, still a work in progress...
</commit_message>
<xml_diff>
--- a/Master_simulation_list.xlsx
+++ b/Master_simulation_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="24540" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25180" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Final set" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="414">
   <si>
     <t>RCE sim</t>
   </si>
@@ -1238,6 +1238,30 @@
   </si>
   <si>
     <t>ts8: day 10</t>
+  </si>
+  <si>
+    <t>CTRLv0qro50000qrhSATqdz5000_nx3072_fx4</t>
+  </si>
+  <si>
+    <t>CTRLv0qro80000qrhSATqdz5000_nx3072_fdiv4</t>
+  </si>
+  <si>
+    <t>CTRLv0qro50000qrhSATqdz5000_nx3072_fx4_lh375</t>
+  </si>
+  <si>
+    <t>CTRLv0qro80000qrhSATqdz5000_nx3072_fdiv4_lh6000</t>
+  </si>
+  <si>
+    <t>HOPRU2N</t>
+  </si>
+  <si>
+    <t>HOPRU9N</t>
+  </si>
+  <si>
+    <t>HOPRU10N</t>
+  </si>
+  <si>
+    <t>HOPRU11N</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1345,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2567">
+  <cellStyleXfs count="2581">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3917,14 +3955,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2567">
+  <cellStyles count="2581">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5208,6 +5246,13 @@
     <cellStyle name="Followed Hyperlink" xfId="2562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2580" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6491,6 +6536,13 @@
     <cellStyle name="Hyperlink" xfId="2561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2579" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6822,8 +6874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C167" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G214" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6851,13 +6903,13 @@
       <c r="I2" t="s">
         <v>152</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
@@ -10894,7 +10946,7 @@
       <c r="A205" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="F205" s="13" t="s">
+      <c r="F205" s="12" t="s">
         <v>404</v>
       </c>
     </row>
@@ -10974,11 +11026,11 @@
       </c>
     </row>
     <row r="209" spans="2:8">
-      <c r="B209" s="1" t="s">
-        <v>131</v>
+      <c r="B209" t="s">
+        <v>117</v>
       </c>
       <c r="C209">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D209">
         <v>48</v>
@@ -11002,23 +11054,96 @@
       <c r="H210" s="4"/>
     </row>
     <row r="211" spans="2:8">
-      <c r="F211" s="4"/>
-      <c r="G211" s="4"/>
-      <c r="H211" s="4"/>
+      <c r="B211" t="s">
+        <v>117</v>
+      </c>
+      <c r="C211">
+        <v>15</v>
+      </c>
+      <c r="D211">
+        <v>48</v>
+      </c>
+      <c r="E211" t="s">
+        <v>146</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="G211" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="H211" s="4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="212" spans="2:8">
-      <c r="F212" s="4"/>
-      <c r="G212" s="4"/>
-      <c r="H212" s="4"/>
+      <c r="B212" t="s">
+        <v>117</v>
+      </c>
+      <c r="C212">
+        <v>15</v>
+      </c>
+      <c r="D212">
+        <v>48</v>
+      </c>
+      <c r="E212" t="s">
+        <v>146</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="G212" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="H212" s="4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="213" spans="2:8">
-      <c r="F213" s="4"/>
-      <c r="G213" s="4"/>
-      <c r="H213" s="4"/>
+      <c r="B213" t="s">
+        <v>117</v>
+      </c>
+      <c r="C213">
+        <v>15</v>
+      </c>
+      <c r="D213">
+        <v>48</v>
+      </c>
+      <c r="E213" t="s">
+        <v>146</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="G213" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="H213" s="4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="214" spans="2:8">
-      <c r="G214" s="4"/>
-      <c r="H214" s="4"/>
+      <c r="B214" t="s">
+        <v>117</v>
+      </c>
+      <c r="C214">
+        <v>15</v>
+      </c>
+      <c r="D214">
+        <v>48</v>
+      </c>
+      <c r="E214" t="s">
+        <v>146</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="G214" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="H214" s="4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="215" spans="2:8">
       <c r="F215" s="4"/>

</xml_diff>

<commit_message>
drc; Updated some small aesthetics in the output plots of TC_stats_plot.m and TC_structure_ts.m
</commit_message>
<xml_diff>
--- a/Master_simulation_list.xlsx
+++ b/Master_simulation_list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25180" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25180" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Final set" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="412">
   <si>
     <t>RCE sim</t>
   </si>
@@ -976,9 +976,6 @@
     <t>CTRLv0qrhSATqdz5000_nx3072_usfc10_drag</t>
   </si>
   <si>
-    <t>HOPRU3N</t>
-  </si>
-  <si>
     <t>different (and worse)!</t>
   </si>
   <si>
@@ -1204,9 +1201,6 @@
     <t>HOPRU14N</t>
   </si>
   <si>
-    <t>HOPRU18N</t>
-  </si>
-  <si>
     <t>TRANSIENT</t>
   </si>
   <si>
@@ -1252,16 +1246,16 @@
     <t>CTRLv0qro80000qrhSATqdz5000_nx3072_fdiv4_lh6000</t>
   </si>
   <si>
-    <t>HOPRU2N</t>
-  </si>
-  <si>
-    <t>HOPRU9N</t>
-  </si>
-  <si>
-    <t>HOPRU10N</t>
-  </si>
-  <si>
-    <t>HOPRU11N</t>
+    <t xml:space="preserve">RCE_nx48_SST287.50K_Tthresh200K_usfc3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCE_nx48_SST292.50K_Tthresh200K_usfc3 </t>
+  </si>
+  <si>
+    <t>RU1N</t>
+  </si>
+  <si>
+    <t>RU2N</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2581">
+  <cellStyleXfs count="2605">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3927,8 +3921,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3961,8 +3979,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2581">
+  <cellStyles count="2605">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5253,6 +5272,18 @@
     <cellStyle name="Followed Hyperlink" xfId="2576" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2578" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2604" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6543,6 +6574,18 @@
     <cellStyle name="Hyperlink" xfId="2575" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2577" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2603" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6872,10 +6915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V246"/>
+  <dimension ref="A1:V248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G214" sqref="G214"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8481,22 +8524,10 @@
     </row>
     <row r="84" spans="1:19">
       <c r="B84" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C84" s="7">
-        <v>11</v>
-      </c>
-      <c r="D84">
-        <v>40</v>
-      </c>
-      <c r="E84" t="s">
-        <v>146</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>151</v>
+        <v>408</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>411</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="5"/>
@@ -8505,94 +8536,90 @@
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="2"/>
     </row>
     <row r="85" spans="1:19">
       <c r="B85" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C85">
-        <v>13</v>
+        <v>306</v>
+      </c>
+      <c r="C85" s="7">
+        <v>11</v>
       </c>
       <c r="D85">
         <v>40</v>
       </c>
-      <c r="E85" s="7" t="s">
+      <c r="E85" t="s">
         <v>146</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G85" s="2">
-        <v>40</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>146</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I85" s="2"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
     </row>
     <row r="86" spans="1:19">
       <c r="B86" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C86">
-        <v>13</v>
-      </c>
-      <c r="D86">
-        <v>40</v>
-      </c>
-      <c r="E86" t="s">
-        <v>146</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G86" s="2">
-        <v>40</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>146</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C87">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D87">
-        <v>48</v>
-      </c>
-      <c r="E87" t="s">
+        <v>40</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>54</v>
+        <v>99</v>
+      </c>
+      <c r="G87" s="2">
+        <v>40</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:19">
       <c r="B88" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C88">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D88">
         <v>40</v>
@@ -8601,7 +8628,7 @@
         <v>146</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G88" s="2">
         <v>40</v>
@@ -8616,220 +8643,223 @@
         <v>151</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M88" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="N88" s="2" t="s">
-        <v>281</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:19">
       <c r="B89" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C89">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D89">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E89" t="s">
         <v>146</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G89" s="2">
-        <v>40</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="J89" s="5"/>
-      <c r="K89" s="2" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:19">
       <c r="B90" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C90">
+        <v>16</v>
+      </c>
+      <c r="D90">
+        <v>40</v>
+      </c>
+      <c r="E90" t="s">
+        <v>146</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G90" s="2">
+        <v>40</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="N90" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="B91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C91">
+        <v>17</v>
+      </c>
+      <c r="D91">
+        <v>40</v>
+      </c>
+      <c r="E91" t="s">
+        <v>146</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G91" s="2">
+        <v>40</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="B92" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C90">
+      <c r="C92">
         <v>17.5</v>
       </c>
-      <c r="D90">
+      <c r="D92">
         <v>48</v>
       </c>
-      <c r="E90" t="s">
-        <v>146</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="E92" t="s">
+        <v>146</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G90" s="2">
+      <c r="G92" s="2">
         <v>48</v>
       </c>
-      <c r="H90" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M90" t="s">
+      <c r="H92" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M92" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
-      <c r="A92" t="s">
+    <row r="94" spans="1:19">
+      <c r="A94" t="s">
         <v>43</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C92">
+      <c r="C94">
         <v>8</v>
       </c>
-      <c r="D92">
-        <v>40</v>
-      </c>
-      <c r="E92" t="s">
-        <v>146</v>
-      </c>
-      <c r="F92" s="2" t="s">
+      <c r="D94">
+        <v>40</v>
+      </c>
+      <c r="E94" t="s">
+        <v>146</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G92" s="2">
-        <v>40</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I92" s="2" t="s">
+      <c r="G94" s="2">
+        <v>40</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J92" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K92" s="2" t="s">
+      <c r="J94" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K94" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="L92" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M92" s="2" t="s">
+      <c r="L94" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M94" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="N92" s="2" t="s">
+      <c r="N94" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="O92" s="5" t="s">
+      <c r="O94" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="P92" s="2" t="s">
+      <c r="P94" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="R92" s="2" t="s">
+      <c r="R94" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="S92" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19">
-      <c r="B93" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C93">
-        <v>12</v>
-      </c>
-      <c r="D93">
-        <v>40</v>
-      </c>
-      <c r="E93" t="s">
-        <v>146</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G93" s="2">
-        <v>40</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19">
-      <c r="B94" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C94">
-        <v>15</v>
-      </c>
-      <c r="D94">
-        <v>48</v>
-      </c>
-      <c r="E94" t="s">
-        <v>146</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>54</v>
+      <c r="S94" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:19">
       <c r="B95" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C95">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D95">
-        <v>48</v>
-      </c>
-      <c r="E95" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E95" t="s">
         <v>146</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="G95" s="2">
-        <v>48</v>
-      </c>
-      <c r="H95" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="J95" s="6" t="s">
-        <v>151</v>
+        <v>40</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:19">
       <c r="B96" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C96">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D96">
         <v>48</v>
@@ -8838,171 +8868,141 @@
         <v>146</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22">
+      <c r="B97" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C97">
+        <v>17</v>
+      </c>
+      <c r="D97">
+        <v>48</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G97" s="2">
+        <v>48</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="J97" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22">
+      <c r="B98" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C98">
+        <v>21</v>
+      </c>
+      <c r="D98">
+        <v>48</v>
+      </c>
+      <c r="E98" t="s">
+        <v>146</v>
+      </c>
+      <c r="F98" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G98" s="2">
         <v>48</v>
       </c>
-      <c r="H96" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K96" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="98" spans="1:22">
-      <c r="A98" t="s">
+      <c r="H98" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K98" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22">
+      <c r="A100" t="s">
         <v>44</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C98">
+      <c r="C100">
         <v>13</v>
       </c>
-      <c r="D98">
-        <v>40</v>
-      </c>
-      <c r="E98" t="s">
-        <v>146</v>
-      </c>
-      <c r="F98" s="2" t="s">
+      <c r="D100">
+        <v>40</v>
+      </c>
+      <c r="E100" t="s">
+        <v>146</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G98" s="2">
-        <v>40</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K98" s="2" t="s">
+      <c r="G100" s="2">
+        <v>40</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K100" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="L98" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M98" s="2" t="s">
+      <c r="L100" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M100" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="N98" s="2" t="s">
+      <c r="N100" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="O98" s="2" t="s">
+      <c r="O100" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="P98" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q98" s="2" t="s">
+      <c r="P100" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q100" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="R98" s="2" t="s">
+      <c r="R100" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="S100" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="T100" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="S98" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="T98" s="2" t="s">
+      <c r="U100" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="V100" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="U98" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="V98" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="99" spans="1:22">
-      <c r="B99" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99">
-        <v>14</v>
-      </c>
-      <c r="D99">
-        <v>48</v>
-      </c>
-      <c r="E99" t="s">
-        <v>146</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G99" s="2">
-        <v>40</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J99" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="L99" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M99" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="N99" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="O99" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="100" spans="1:22">
-      <c r="B100" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C100">
-        <v>14</v>
-      </c>
-      <c r="D100">
-        <v>40</v>
-      </c>
-      <c r="E100" t="s">
-        <v>146</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G100" s="2">
-        <v>40</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J100" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:22">
       <c r="B101" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C101">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D101">
         <v>48</v>
@@ -9011,15 +9011,42 @@
         <v>146</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
+      </c>
+      <c r="G101" s="2">
+        <v>40</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N101" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="O101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:22">
       <c r="B102" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C102">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D102">
         <v>40</v>
@@ -9028,7 +9055,7 @@
         <v>146</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G102" s="2">
         <v>40</v>
@@ -9037,7 +9064,7 @@
         <v>146</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="J102" s="5" t="s">
         <v>151</v>
@@ -9048,7 +9075,7 @@
     </row>
     <row r="103" spans="1:22">
       <c r="B103" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C103">
         <v>15</v>
@@ -9060,27 +9087,12 @@
         <v>146</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G103" s="2">
-        <v>40</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J103" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="1:22">
       <c r="B104" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C104">
         <v>15</v>
@@ -9092,100 +9104,103 @@
         <v>146</v>
       </c>
       <c r="F104" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G104" s="2">
+        <v>40</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22">
+      <c r="B105" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C105">
+        <v>15</v>
+      </c>
+      <c r="D105">
+        <v>48</v>
+      </c>
+      <c r="E105" t="s">
+        <v>146</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G105" s="2">
+        <v>40</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22">
+      <c r="B106" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106">
+        <v>15</v>
+      </c>
+      <c r="D106">
+        <v>40</v>
+      </c>
+      <c r="E106" t="s">
+        <v>146</v>
+      </c>
+      <c r="F106" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G104" s="2">
-        <v>40</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I104" s="2" t="s">
+      <c r="G106" s="2">
+        <v>40</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I106" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J104" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="105" spans="1:22">
-      <c r="B105" s="1"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:22">
-      <c r="A106" t="s">
-        <v>310</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C106">
-        <v>13</v>
-      </c>
-      <c r="D106">
-        <v>40</v>
-      </c>
-      <c r="E106" t="s">
-        <v>146</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G106" s="2">
-        <v>40</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I106" s="2"/>
-      <c r="J106" s="5"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
-      <c r="N106" s="2"/>
-      <c r="O106" s="2"/>
-      <c r="P106" s="5"/>
-      <c r="Q106" s="2"/>
+      <c r="J106" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="107" spans="1:22">
-      <c r="B107" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C107">
-        <v>14</v>
-      </c>
-      <c r="D107">
-        <v>48</v>
-      </c>
-      <c r="E107" t="s">
-        <v>146</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="G107" s="2">
-        <v>40</v>
-      </c>
-      <c r="H107" s="6" t="s">
-        <v>151</v>
-      </c>
+      <c r="B107" s="1"/>
       <c r="I107" s="2"/>
       <c r="J107" s="5"/>
       <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-      <c r="N107" s="2"/>
     </row>
     <row r="108" spans="1:22">
+      <c r="A108" t="s">
+        <v>310</v>
+      </c>
       <c r="B108" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C108">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D108">
         <v>40</v>
@@ -9194,7 +9209,7 @@
         <v>146</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G108" s="2">
         <v>40</v>
@@ -9205,13 +9220,19 @@
       <c r="I108" s="2"/>
       <c r="J108" s="5"/>
       <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+      <c r="M108" s="2"/>
+      <c r="N108" s="2"/>
+      <c r="O108" s="2"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="2"/>
     </row>
     <row r="109" spans="1:22">
       <c r="B109" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C109">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D109">
         <v>48</v>
@@ -9220,7 +9241,7 @@
         <v>146</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G109" s="2">
         <v>40</v>
@@ -9228,13 +9249,19 @@
       <c r="H109" s="6" t="s">
         <v>151</v>
       </c>
+      <c r="I109" s="2"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
     </row>
     <row r="110" spans="1:22">
       <c r="B110" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C110">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D110">
         <v>40</v>
@@ -9243,7 +9270,7 @@
         <v>146</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G110" s="2">
         <v>40</v>
@@ -9257,7 +9284,7 @@
     </row>
     <row r="111" spans="1:22">
       <c r="B111" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C111">
         <v>15</v>
@@ -9269,7 +9296,7 @@
         <v>146</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G111" s="2">
         <v>40</v>
@@ -9277,13 +9304,10 @@
       <c r="H111" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="I111" s="2"/>
-      <c r="J111" s="5"/>
-      <c r="K111" s="2"/>
     </row>
     <row r="112" spans="1:22">
       <c r="B112" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C112">
         <v>15</v>
@@ -9295,7 +9319,7 @@
         <v>146</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G112" s="2">
         <v>40</v>
@@ -9307,76 +9331,64 @@
       <c r="J112" s="5"/>
       <c r="K112" s="2"/>
     </row>
+    <row r="113" spans="1:15">
+      <c r="B113" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C113">
+        <v>15</v>
+      </c>
+      <c r="D113">
+        <v>48</v>
+      </c>
+      <c r="E113" t="s">
+        <v>146</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G113" s="2">
+        <v>40</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I113" s="2"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="2"/>
+    </row>
     <row r="114" spans="1:15">
-      <c r="A114" t="s">
-        <v>45</v>
-      </c>
       <c r="B114" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C114">
         <v>15</v>
       </c>
       <c r="D114">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E114" t="s">
         <v>146</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>179</v>
+        <v>317</v>
       </c>
       <c r="G114" s="2">
         <v>40</v>
       </c>
-      <c r="H114" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J114" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15">
-      <c r="B115" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C115">
-        <v>15</v>
-      </c>
-      <c r="D115">
-        <v>48</v>
-      </c>
-      <c r="E115" t="s">
-        <v>146</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G115" s="2">
-        <v>40</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J115" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="H114" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I114" s="2"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="2"/>
     </row>
     <row r="116" spans="1:15">
+      <c r="A116" t="s">
+        <v>45</v>
+      </c>
       <c r="B116" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="C116">
         <v>15</v>
@@ -9388,15 +9400,30 @@
         <v>146</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>54</v>
+        <v>179</v>
+      </c>
+      <c r="G116" s="2">
+        <v>40</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:15">
       <c r="B117" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C117">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D117">
         <v>48</v>
@@ -9405,135 +9432,135 @@
         <v>146</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G117" s="2">
-        <v>48</v>
-      </c>
-      <c r="H117" s="8" t="s">
-        <v>146</v>
+        <v>40</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="J117" s="5" t="s">
         <v>151</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:15">
       <c r="B118" s="1" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C118">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D118">
         <v>48</v>
       </c>
-      <c r="E118" s="7" t="s">
+      <c r="E118" t="s">
         <v>146</v>
       </c>
       <c r="F118" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="B119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C119">
+        <v>14</v>
+      </c>
+      <c r="D119">
+        <v>48</v>
+      </c>
+      <c r="E119" t="s">
+        <v>146</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G119" s="2">
+        <v>48</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J119" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="B120" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C120">
+        <v>13</v>
+      </c>
+      <c r="D120">
+        <v>48</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G118" s="2">
+      <c r="G120" s="2">
         <v>48</v>
       </c>
-      <c r="H118" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I118" s="5" t="s">
+      <c r="H120" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I120" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="J118" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="K118" t="s">
+      <c r="J120" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K120" t="s">
         <v>278</v>
       </c>
-      <c r="L118" t="s">
-        <v>146</v>
-      </c>
-      <c r="M118" t="s">
+      <c r="L120" t="s">
+        <v>146</v>
+      </c>
+      <c r="M120" t="s">
         <v>288</v>
       </c>
-      <c r="N118" t="s">
+      <c r="N120" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="120" spans="1:15">
-      <c r="A120" t="s">
+    <row r="122" spans="1:15">
+      <c r="A122" t="s">
         <v>46</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>117</v>
       </c>
-      <c r="C120">
+      <c r="C122">
         <v>15</v>
       </c>
-      <c r="D120">
-        <v>40</v>
-      </c>
-      <c r="E120" t="s">
-        <v>146</v>
-      </c>
-      <c r="F120" s="2" t="s">
+      <c r="D122">
+        <v>40</v>
+      </c>
+      <c r="E122" t="s">
+        <v>146</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G120" s="2">
-        <v>40</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I120" s="2" t="s">
+      <c r="G122" s="2">
+        <v>40</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I122" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="J120" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15">
-      <c r="F121" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G121" s="2">
-        <v>40</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I121" t="s">
-        <v>175</v>
-      </c>
-      <c r="J121" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="L121" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M121" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N121" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15">
-      <c r="F122" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G122" s="2">
-        <v>40</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I122" t="s">
-        <v>146</v>
       </c>
       <c r="J122" s="5" t="s">
         <v>151</v>
@@ -9544,12 +9571,36 @@
     </row>
     <row r="123" spans="1:15">
       <c r="F123" s="2" t="s">
-        <v>54</v>
+        <v>112</v>
+      </c>
+      <c r="G123" s="2">
+        <v>40</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I123" t="s">
+        <v>175</v>
+      </c>
+      <c r="J123" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N123" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="124" spans="1:15">
       <c r="F124" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G124" s="2">
         <v>40</v>
@@ -9558,149 +9609,147 @@
         <v>146</v>
       </c>
       <c r="I124" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="J124" s="5" t="s">
         <v>151</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="L124" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M124" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="N124" s="2" t="s">
-        <v>292</v>
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="1:15">
       <c r="F125" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="F126" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G126" s="2">
+        <v>40</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I126" t="s">
+        <v>176</v>
+      </c>
+      <c r="J126" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="F127" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G125" s="2">
-        <v>40</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I125" t="s">
+      <c r="G127" s="2">
+        <v>40</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I127" t="s">
         <v>177</v>
       </c>
-      <c r="J125" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K125" s="2" t="s">
+      <c r="J127" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K127" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="L127" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="M125" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N125" s="2" t="s">
+      <c r="M127" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N127" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="126" spans="1:15">
-      <c r="F126" s="3" t="s">
+    <row r="128" spans="1:15">
+      <c r="F128" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G126" s="2">
-        <v>40</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I126" t="s">
+      <c r="G128" s="2">
+        <v>40</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I128" t="s">
         <v>178</v>
       </c>
-      <c r="J126" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K126" s="2" t="s">
+      <c r="J128" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="K128" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="O126" t="s">
+      <c r="O128" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="127" spans="1:15">
-      <c r="A127" t="s">
+    <row r="129" spans="1:14">
+      <c r="A129" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="128" spans="1:15">
-      <c r="A128" t="s">
-        <v>187</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C128">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="D128">
-        <v>48</v>
-      </c>
-      <c r="E128" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G128" s="2">
-        <v>48</v>
-      </c>
-      <c r="J128" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="K128" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14">
-      <c r="B129" s="1"/>
-      <c r="C129">
-        <f>C128/$C$130</f>
-        <v>1.2071428571428571</v>
-      </c>
-      <c r="E129" s="7"/>
-      <c r="F129" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J129" s="6" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="130" spans="1:14">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="C130">
-        <v>14</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D130">
         <v>48</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>54</v>
+        <v>191</v>
+      </c>
+      <c r="G130" s="2">
+        <v>48</v>
+      </c>
+      <c r="J130" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:14">
       <c r="B131" s="1"/>
       <c r="C131">
-        <f>C130/$C$130</f>
-        <v>1</v>
+        <f>C130/$C$132</f>
+        <v>1.2071428571428571</v>
+      </c>
+      <c r="E131" s="7"/>
+      <c r="F131" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J131" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="132" spans="1:14">
@@ -9708,51 +9757,26 @@
         <v>185</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>192</v>
+        <v>117</v>
       </c>
       <c r="C132">
-        <v>11.4</v>
+        <v>14</v>
       </c>
       <c r="D132">
         <v>48</v>
       </c>
-      <c r="E132" s="7" t="s">
+      <c r="E132" t="s">
         <v>146</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G132" s="2">
-        <v>40</v>
-      </c>
-      <c r="J132" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K132" t="s">
-        <v>296</v>
-      </c>
-      <c r="L132" t="s">
-        <v>146</v>
-      </c>
-      <c r="M132" t="s">
-        <v>297</v>
-      </c>
-      <c r="N132" t="s">
-        <v>298</v>
+        <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:14">
       <c r="B133" s="1"/>
       <c r="C133">
-        <f>C132/$C$130</f>
-        <v>0.81428571428571428</v>
-      </c>
-      <c r="E133" s="7"/>
-      <c r="F133" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J133" s="5" t="s">
-        <v>151</v>
+        <f>C132/$C$132</f>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:14">
@@ -9760,10 +9784,10 @@
         <v>185</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C134">
-        <v>8.4</v>
+        <v>11.4</v>
       </c>
       <c r="D134">
         <v>48</v>
@@ -9772,36 +9796,36 @@
         <v>146</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G134" s="2">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J134" s="5" t="s">
         <v>151</v>
       </c>
       <c r="K134" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="L134" t="s">
-        <v>299</v>
+        <v>146</v>
       </c>
       <c r="M134" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="N134" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="135" spans="1:14">
       <c r="B135" s="1"/>
       <c r="C135">
-        <f>C134/$C$130</f>
-        <v>0.6</v>
+        <f>C134/$C$132</f>
+        <v>0.81428571428571428</v>
       </c>
       <c r="E135" s="7"/>
       <c r="F135" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J135" s="5" t="s">
         <v>151</v>
@@ -9809,39 +9833,51 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C136">
-        <v>6.2</v>
+        <v>8.4</v>
       </c>
       <c r="D136">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G136" s="2">
         <v>32</v>
       </c>
       <c r="J136" s="5" t="s">
         <v>151</v>
+      </c>
+      <c r="K136" t="s">
+        <v>300</v>
+      </c>
+      <c r="L136" t="s">
+        <v>299</v>
+      </c>
+      <c r="M136" t="s">
+        <v>301</v>
+      </c>
+      <c r="N136" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="137" spans="1:14">
       <c r="B137" s="1"/>
       <c r="C137">
-        <f>C136/$C$130</f>
-        <v>0.44285714285714289</v>
+        <f>C136/$C$132</f>
+        <v>0.6</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J137" s="5" t="s">
         <v>151</v>
@@ -9849,13 +9885,13 @@
     </row>
     <row r="138" spans="1:14">
       <c r="A138" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C138">
-        <v>3.6</v>
+        <v>6.2</v>
       </c>
       <c r="D138">
         <v>40</v>
@@ -9864,10 +9900,10 @@
         <v>146</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G138" s="2">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J138" s="5" t="s">
         <v>151</v>
@@ -9876,12 +9912,12 @@
     <row r="139" spans="1:14">
       <c r="B139" s="1"/>
       <c r="C139">
-        <f>C138/$C$130</f>
-        <v>0.25714285714285717</v>
+        <f>C138/$C$132</f>
+        <v>0.44285714285714289</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J139" s="5" t="s">
         <v>151</v>
@@ -9892,10 +9928,10 @@
         <v>185</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C140">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="D140">
         <v>40</v>
@@ -9904,7 +9940,7 @@
         <v>146</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G140" s="2">
         <v>24</v>
@@ -9916,70 +9952,76 @@
     <row r="141" spans="1:14">
       <c r="B141" s="1"/>
       <c r="C141">
-        <f>C140/$C$130</f>
-        <v>0.18571428571428572</v>
+        <f>C140/$C$132</f>
+        <v>0.25714285714285717</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J141" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
+      <c r="A142" t="s">
+        <v>185</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C142">
+        <v>2.6</v>
+      </c>
+      <c r="D142">
+        <v>40</v>
+      </c>
+      <c r="E142" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G142" s="2">
+        <v>24</v>
+      </c>
+      <c r="J142" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="B143" s="1"/>
+      <c r="C143">
+        <f>C142/$C$132</f>
+        <v>0.18571428571428572</v>
+      </c>
+      <c r="E143" s="7"/>
+      <c r="F143" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J141" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14">
-      <c r="B142" s="1"/>
-      <c r="E142" s="5"/>
-    </row>
-    <row r="143" spans="1:14">
-      <c r="A143" t="s">
-        <v>193</v>
-      </c>
-      <c r="E143" s="7"/>
+      <c r="J143" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="144" spans="1:14">
-      <c r="A144" t="s">
-        <v>194</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D144">
-        <v>56</v>
-      </c>
-      <c r="E144" s="7" t="s">
-        <v>170</v>
-      </c>
+      <c r="B144" s="1"/>
+      <c r="E144" s="5"/>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" t="s">
-        <v>197</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C145">
-        <v>20</v>
-      </c>
-      <c r="D145">
-        <v>48</v>
-      </c>
-      <c r="E145" s="7" t="s">
-        <v>170</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="E145" s="7"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C146">
-        <v>22</v>
+        <v>199</v>
       </c>
       <c r="D146">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>170</v>
@@ -9987,47 +10029,47 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C147">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D147">
         <v>48</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C148">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D148">
         <v>48</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C149">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D149">
         <v>48</v>
@@ -10038,13 +10080,13 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C150">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D150">
         <v>48</v>
@@ -10055,16 +10097,16 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C151">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D151">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E151" s="7" t="s">
         <v>146</v>
@@ -10072,16 +10114,16 @@
     </row>
     <row r="152" spans="1:12">
       <c r="A152" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C152">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D152">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E152" s="7" t="s">
         <v>146</v>
@@ -10089,13 +10131,13 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C153">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D153">
         <v>40</v>
@@ -10106,13 +10148,13 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C154">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D154">
         <v>40</v>
@@ -10123,885 +10165,870 @@
     </row>
     <row r="155" spans="1:12">
       <c r="A155" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C155">
         <v>3</v>
       </c>
       <c r="D155">
+        <v>40</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" t="s">
+        <v>202</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C156">
+        <v>3</v>
+      </c>
+      <c r="D156">
+        <v>40</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157" t="s">
+        <v>188</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C157">
+        <v>3</v>
+      </c>
+      <c r="D157">
         <v>24</v>
       </c>
-      <c r="E155" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12">
-      <c r="B156" s="1"/>
-      <c r="E156" s="7"/>
+      <c r="E157" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="158" spans="1:12">
-      <c r="A158" t="s">
+      <c r="B158" s="1"/>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="A160" t="s">
         <v>49</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B160" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C158">
+      <c r="C160">
         <v>21</v>
       </c>
-      <c r="D158">
+      <c r="D160">
         <v>48</v>
       </c>
-      <c r="E158" t="s">
-        <v>146</v>
-      </c>
-      <c r="F158" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="G158" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="H158" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K158" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="L158" s="3" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12">
-      <c r="F159" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="G159" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="H159" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="K159" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="L159" s="3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12">
-      <c r="B160" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C160">
-        <v>8</v>
-      </c>
-      <c r="D160">
-        <v>40</v>
-      </c>
       <c r="E160" t="s">
         <v>146</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G160" s="9" t="s">
-        <v>151</v>
+        <v>366</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I160" t="s">
-        <v>365</v>
+        <v>370</v>
+      </c>
+      <c r="K160" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="L160" s="3" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="161" spans="2:12">
       <c r="F161" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G161" s="10" t="s">
-        <v>151</v>
+        <v>366</v>
       </c>
       <c r="H161" s="4" t="s">
-        <v>325</v>
+        <v>371</v>
+      </c>
+      <c r="K161" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="L161" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="162" spans="2:12">
-      <c r="G162" s="3"/>
-      <c r="H162" s="3"/>
+      <c r="B162" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C162">
+        <v>8</v>
+      </c>
+      <c r="D162">
+        <v>40</v>
+      </c>
+      <c r="E162" t="s">
+        <v>146</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G162" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="I162" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="163" spans="2:12">
-      <c r="B163" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C163">
-        <v>21</v>
-      </c>
-      <c r="D163">
-        <v>48</v>
-      </c>
-      <c r="E163" t="s">
-        <v>146</v>
-      </c>
       <c r="F163" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G163" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H163" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="164" spans="2:12">
-      <c r="F164" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="G164" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="H164" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="K164" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="L164" s="3" t="s">
-        <v>387</v>
-      </c>
+      <c r="G164" s="3"/>
+      <c r="H164" s="3"/>
     </row>
     <row r="165" spans="2:12">
       <c r="B165" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C165">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D165">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E165" t="s">
         <v>146</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G165" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="G165" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H165" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="166" spans="2:12">
       <c r="F166" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G166" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H166" s="4" t="s">
-        <v>325</v>
+        <v>332</v>
+      </c>
+      <c r="G166" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K166" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="L166" s="3" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="167" spans="2:12">
-      <c r="G167" s="3"/>
-      <c r="H167" s="3"/>
+      <c r="B167" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C167">
+        <v>8</v>
+      </c>
+      <c r="D167">
+        <v>40</v>
+      </c>
+      <c r="E167" t="s">
+        <v>146</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G167" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H167" s="4" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="168" spans="2:12">
-      <c r="B168" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C168">
-        <v>21</v>
-      </c>
-      <c r="D168">
-        <v>48</v>
-      </c>
-      <c r="E168" t="s">
-        <v>146</v>
-      </c>
       <c r="F168" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G168" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H168" s="3" t="s">
-        <v>325</v>
+      <c r="H168" s="4" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="169" spans="2:12">
-      <c r="F169" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G169" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="H169" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="K169" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="L169" s="3" t="s">
-        <v>389</v>
-      </c>
+      <c r="G169" s="3"/>
+      <c r="H169" s="3"/>
     </row>
     <row r="170" spans="2:12">
       <c r="B170" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C170">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D170">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E170" t="s">
         <v>146</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G170" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="171" spans="2:12">
       <c r="F171" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G171" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H171" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="L171" s="3"/>
+        <v>366</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="K171" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="L171" s="3" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="172" spans="2:12">
-      <c r="G172" s="3"/>
-      <c r="H172" s="3"/>
+      <c r="B172" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C172">
+        <v>8</v>
+      </c>
+      <c r="D172">
+        <v>40</v>
+      </c>
+      <c r="E172" t="s">
+        <v>146</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G172" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="173" spans="2:12">
-      <c r="B173" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C173">
-        <v>21</v>
-      </c>
-      <c r="D173">
-        <v>48</v>
-      </c>
-      <c r="E173" t="s">
-        <v>146</v>
-      </c>
       <c r="F173" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G173" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H173" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="H173" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="L173" s="3"/>
     </row>
     <row r="174" spans="2:12">
-      <c r="F174" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="G174" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H174" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="G174" s="3"/>
+      <c r="H174" s="3"/>
     </row>
     <row r="175" spans="2:12">
       <c r="B175" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C175">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D175">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E175" t="s">
         <v>146</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G175" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H175" s="4" t="s">
-        <v>325</v>
+      <c r="H175" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="176" spans="2:12">
       <c r="F176" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G176" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H176" s="4" t="s">
-        <v>325</v>
+        <v>340</v>
+      </c>
+      <c r="G176" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="177" spans="2:12">
-      <c r="G177" s="3"/>
-      <c r="H177" s="3"/>
+      <c r="B177" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C177">
+        <v>8</v>
+      </c>
+      <c r="D177">
+        <v>40</v>
+      </c>
+      <c r="E177" t="s">
+        <v>146</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="G177" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H177" s="4" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="178" spans="2:12">
-      <c r="B178" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C178">
-        <v>21</v>
-      </c>
-      <c r="D178">
-        <v>48</v>
-      </c>
-      <c r="E178" t="s">
-        <v>146</v>
-      </c>
       <c r="F178" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="G178" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G178" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H178" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H178" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="L178" s="3"/>
-    </row>
-    <row r="179" spans="2:12" ht="18">
-      <c r="F179" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G179" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H179" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="L179" s="11"/>
+    </row>
+    <row r="179" spans="2:12">
+      <c r="G179" s="3"/>
+      <c r="H179" s="3"/>
     </row>
     <row r="180" spans="2:12">
       <c r="B180" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C180">
+        <v>21</v>
+      </c>
+      <c r="D180">
+        <v>48</v>
+      </c>
+      <c r="E180" t="s">
+        <v>146</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G180" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H180" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="L180" s="3"/>
+    </row>
+    <row r="181" spans="2:12" ht="18">
+      <c r="F181" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="G181" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H181" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="L181" s="11"/>
+    </row>
+    <row r="182" spans="2:12">
+      <c r="B182" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C180">
+      <c r="C182">
         <v>8</v>
       </c>
-      <c r="D180">
-        <v>40</v>
-      </c>
-      <c r="E180" t="s">
-        <v>146</v>
-      </c>
-      <c r="F180" s="3" t="s">
+      <c r="D182">
+        <v>40</v>
+      </c>
+      <c r="E182" t="s">
+        <v>146</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G182" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H182" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="183" spans="2:12">
+      <c r="F183" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G180" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H180" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="181" spans="2:12">
-      <c r="F181" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="G181" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H181" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="182" spans="2:12">
-      <c r="G182" s="3"/>
-      <c r="H182" s="3"/>
-    </row>
-    <row r="183" spans="2:12">
-      <c r="B183" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C183">
-        <v>21</v>
-      </c>
-      <c r="D183">
-        <v>48</v>
-      </c>
-      <c r="E183" t="s">
-        <v>146</v>
-      </c>
-      <c r="F183" s="3" t="s">
-        <v>348</v>
-      </c>
       <c r="G183" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H183" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H183" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="K183" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="L183" s="3" t="s">
-        <v>381</v>
-      </c>
     </row>
     <row r="184" spans="2:12">
-      <c r="F184" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G184" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H184" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
     </row>
     <row r="185" spans="2:12">
       <c r="B185" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C185">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D185">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E185" t="s">
         <v>146</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G185" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H185" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K185" s="5" t="s">
-        <v>322</v>
+        <v>381</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="186" spans="2:12">
       <c r="F186" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G186" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H186" s="4" t="s">
-        <v>325</v>
+      <c r="H186" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="187" spans="2:12">
-      <c r="F187" s="3"/>
-      <c r="G187" s="3"/>
-      <c r="H187" s="3"/>
+      <c r="B187" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C187">
+        <v>8</v>
+      </c>
+      <c r="D187">
+        <v>40</v>
+      </c>
+      <c r="E187" t="s">
+        <v>146</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G187" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H187" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="K187" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="L187" s="3" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="188" spans="2:12">
-      <c r="B188" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C188">
-        <v>21</v>
-      </c>
-      <c r="D188">
-        <v>48</v>
-      </c>
-      <c r="E188" t="s">
-        <v>146</v>
-      </c>
-      <c r="F188" s="4" t="s">
-        <v>352</v>
+      <c r="F188" s="3" t="s">
+        <v>350</v>
       </c>
       <c r="G188" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H188" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H188" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="K188" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="L188" s="4" t="s">
-        <v>383</v>
-      </c>
     </row>
     <row r="189" spans="2:12">
-      <c r="F189" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="G189" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H189" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
     </row>
     <row r="190" spans="2:12">
       <c r="B190" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C190">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D190">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E190" t="s">
         <v>146</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G190" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K190" s="5" t="s">
-        <v>304</v>
+        <v>383</v>
       </c>
       <c r="L190" s="4" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="191" spans="2:12">
       <c r="F191" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="G191" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H191" s="2" t="s">
-        <v>325</v>
+        <v>352</v>
+      </c>
+      <c r="G191" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H191" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="192" spans="2:12">
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
+      <c r="B192" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C192">
+        <v>8</v>
+      </c>
+      <c r="D192">
+        <v>40</v>
+      </c>
+      <c r="E192" t="s">
+        <v>146</v>
+      </c>
+      <c r="F192" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G192" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H192" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="K192" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L192" s="4" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="193" spans="1:16">
-      <c r="B193" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C193">
-        <v>21</v>
-      </c>
-      <c r="D193">
-        <v>48</v>
-      </c>
-      <c r="E193" t="s">
-        <v>146</v>
-      </c>
       <c r="F193" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="G193" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="G193" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H193" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="H193" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="I193" t="s">
-        <v>326</v>
-      </c>
-      <c r="K193" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="L193" s="4" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="194" spans="1:16">
-      <c r="F194" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="G194" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="H194" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="K194" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="L194" s="4" t="s">
-        <v>390</v>
-      </c>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3"/>
     </row>
     <row r="195" spans="1:16">
       <c r="B195" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C195">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D195">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E195" t="s">
         <v>146</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G195" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I195" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K195" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L195" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="M195" t="s">
-        <v>374</v>
-      </c>
-      <c r="O195" t="s">
-        <v>366</v>
-      </c>
-      <c r="P195" s="4" t="s">
-        <v>67</v>
+        <v>375</v>
       </c>
     </row>
     <row r="196" spans="1:16">
       <c r="F196" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G196" s="9" t="s">
-        <v>151</v>
+        <v>366</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>325</v>
+        <v>369</v>
       </c>
       <c r="K196" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L196" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="M196" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
     </row>
     <row r="197" spans="1:16">
-      <c r="F197" s="3"/>
-      <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
-      <c r="O197" s="7" t="s">
-        <v>366</v>
+      <c r="B197" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C197">
+        <v>8</v>
+      </c>
+      <c r="D197">
+        <v>40</v>
+      </c>
+      <c r="E197" t="s">
+        <v>146</v>
+      </c>
+      <c r="F197" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="G197" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H197" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I197" t="s">
+        <v>326</v>
+      </c>
+      <c r="K197" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L197" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="M197" t="s">
+        <v>373</v>
+      </c>
+      <c r="O197" t="s">
+        <v>365</v>
       </c>
       <c r="P197" s="4" t="s">
-        <v>368</v>
+        <v>67</v>
       </c>
     </row>
     <row r="198" spans="1:16">
-      <c r="B198" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C198">
-        <v>21</v>
-      </c>
-      <c r="D198">
-        <v>48</v>
-      </c>
-      <c r="E198" t="s">
-        <v>146</v>
-      </c>
       <c r="F198" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G198" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H198" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="H198" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="K198" s="5" t="s">
-        <v>392</v>
+        <v>151</v>
       </c>
       <c r="L198" s="4" t="s">
-        <v>385</v>
+        <v>379</v>
+      </c>
+      <c r="M198" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="199" spans="1:16">
-      <c r="F199" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="G199" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H199" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="K199" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="L199" s="4" t="s">
-        <v>391</v>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="3"/>
+      <c r="O199" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="P199" s="4" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="200" spans="1:16">
       <c r="B200" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C200">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D200">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E200" t="s">
         <v>146</v>
       </c>
       <c r="F200" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="G200" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="H200" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G200" s="9" t="s">
         <v>323</v>
       </c>
+      <c r="H200" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="K200" s="5" t="s">
-        <v>318</v>
+        <v>391</v>
       </c>
       <c r="L200" s="4" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
     </row>
     <row r="201" spans="1:16">
       <c r="F201" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="G201" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H201" s="4" t="s">
-        <v>325</v>
+        <v>360</v>
+      </c>
+      <c r="G201" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H201" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="K201" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="L201" s="4" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="202" spans="1:16">
-      <c r="G202" s="4"/>
-      <c r="H202" s="4"/>
+      <c r="B202" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C202">
+        <v>8</v>
+      </c>
+      <c r="D202">
+        <v>40</v>
+      </c>
+      <c r="E202" t="s">
+        <v>146</v>
+      </c>
+      <c r="F202" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="G202" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H202" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="K202" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L202" s="4" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="203" spans="1:16">
-      <c r="G203" s="4"/>
-      <c r="H203" s="4"/>
+      <c r="F203" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G203" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H203" s="4" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="204" spans="1:16">
-      <c r="A204" s="5" t="s">
+      <c r="G204" s="4"/>
+      <c r="H204" s="4"/>
+    </row>
+    <row r="205" spans="1:16">
+      <c r="G205" s="4"/>
+      <c r="H205" s="4"/>
+    </row>
+    <row r="206" spans="1:16">
+      <c r="A206" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B204" s="5" t="s">
+      <c r="B206" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C204" s="5" t="s">
+      <c r="C206" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D204" s="5" t="s">
+      <c r="D206" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E204" s="5" t="s">
+      <c r="E206" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F204" s="6" t="s">
+      <c r="F206" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G204" s="6"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="5"/>
-    </row>
-    <row r="205" spans="1:16">
-      <c r="A205" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="F205" s="12" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="206" spans="1:16">
-      <c r="A206" t="s">
-        <v>397</v>
-      </c>
-      <c r="B206" t="s">
-        <v>117</v>
-      </c>
-      <c r="C206">
-        <v>15</v>
-      </c>
-      <c r="D206">
-        <v>48</v>
-      </c>
-      <c r="E206" t="s">
-        <v>146</v>
-      </c>
-      <c r="F206" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G206" s="5" t="s">
-        <v>396</v>
-      </c>
+      <c r="G206" s="6"/>
+      <c r="H206" s="6"/>
+      <c r="I206" s="5"/>
     </row>
     <row r="207" spans="1:16">
-      <c r="A207" t="s">
-        <v>398</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C207">
-        <v>8</v>
-      </c>
-      <c r="D207">
-        <v>40</v>
-      </c>
-      <c r="E207" t="s">
-        <v>146</v>
-      </c>
-      <c r="F207" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="G207" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H207" s="4" t="s">
-        <v>403</v>
+      <c r="A207" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F207" s="12" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="208" spans="1:16">
       <c r="A208" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B208" t="s">
         <v>117</v>
@@ -11016,44 +11043,65 @@
         <v>146</v>
       </c>
       <c r="F208" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="G208" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H208" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="209" spans="2:8">
-      <c r="B209" t="s">
+        <v>54</v>
+      </c>
+      <c r="G208" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" t="s">
+        <v>396</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C209">
+        <v>8</v>
+      </c>
+      <c r="D209">
+        <v>40</v>
+      </c>
+      <c r="E209" t="s">
+        <v>146</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G209" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H209" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
+      <c r="A210" t="s">
+        <v>397</v>
+      </c>
+      <c r="B210" t="s">
         <v>117</v>
       </c>
-      <c r="C209">
+      <c r="C210">
         <v>15</v>
       </c>
-      <c r="D209">
+      <c r="D210">
         <v>48</v>
       </c>
-      <c r="E209" t="s">
-        <v>146</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="G209" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H209" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="210" spans="2:8">
-      <c r="F210" s="4"/>
-      <c r="G210" s="4"/>
-      <c r="H210" s="4"/>
-    </row>
-    <row r="211" spans="2:8">
+      <c r="E210" t="s">
+        <v>146</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G210" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H210" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
       <c r="B211" t="s">
         <v>117</v>
       </c>
@@ -11067,39 +11115,21 @@
         <v>146</v>
       </c>
       <c r="F211" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G211" s="10" t="s">
-        <v>410</v>
+        <v>151</v>
       </c>
       <c r="H211" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="212" spans="2:8">
-      <c r="B212" t="s">
-        <v>117</v>
-      </c>
-      <c r="C212">
-        <v>15</v>
-      </c>
-      <c r="D212">
-        <v>48</v>
-      </c>
-      <c r="E212" t="s">
-        <v>146</v>
-      </c>
-      <c r="F212" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="G212" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="H212" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="213" spans="2:8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8">
+      <c r="F212" s="4"/>
+      <c r="G212" s="4"/>
+      <c r="H212" s="4"/>
+    </row>
+    <row r="213" spans="1:8">
       <c r="B213" t="s">
         <v>117</v>
       </c>
@@ -11113,16 +11143,16 @@
         <v>146</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G213" s="10" t="s">
-        <v>413</v>
+        <v>151</v>
       </c>
       <c r="H213" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="214" spans="2:8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8">
       <c r="B214" t="s">
         <v>117</v>
       </c>
@@ -11136,55 +11166,93 @@
         <v>146</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="G214" s="10" t="s">
-        <v>412</v>
+        <v>151</v>
       </c>
       <c r="H214" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="215" spans="2:8">
-      <c r="F215" s="4"/>
-      <c r="G215" s="4"/>
-      <c r="H215" s="4"/>
-    </row>
-    <row r="216" spans="2:8">
-      <c r="F216" s="4"/>
-      <c r="G216" s="4"/>
-      <c r="H216" s="4"/>
-    </row>
-    <row r="217" spans="2:8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8">
+      <c r="B215" t="s">
+        <v>117</v>
+      </c>
+      <c r="C215">
+        <v>15</v>
+      </c>
+      <c r="D215">
+        <v>48</v>
+      </c>
+      <c r="E215" t="s">
+        <v>146</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="G215" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H215" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8">
+      <c r="B216" t="s">
+        <v>117</v>
+      </c>
+      <c r="C216">
+        <v>15</v>
+      </c>
+      <c r="D216">
+        <v>48</v>
+      </c>
+      <c r="E216" t="s">
+        <v>146</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="G216" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H216" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8">
       <c r="F217" s="4"/>
       <c r="G217" s="4"/>
       <c r="H217" s="4"/>
     </row>
-    <row r="218" spans="2:8">
+    <row r="218" spans="1:8">
+      <c r="F218" s="4"/>
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
     </row>
-    <row r="219" spans="2:8">
+    <row r="219" spans="1:8">
+      <c r="F219" s="4"/>
       <c r="G219" s="4"/>
       <c r="H219" s="4"/>
     </row>
-    <row r="220" spans="2:8">
+    <row r="220" spans="1:8">
       <c r="G220" s="4"/>
       <c r="H220" s="4"/>
     </row>
-    <row r="221" spans="2:8">
-      <c r="G221" s="3"/>
-      <c r="H221" s="3"/>
-    </row>
-    <row r="222" spans="2:8">
+    <row r="221" spans="1:8">
+      <c r="G221" s="4"/>
+      <c r="H221" s="4"/>
+    </row>
+    <row r="222" spans="1:8">
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
     </row>
-    <row r="223" spans="2:8">
-      <c r="G223" s="4"/>
-      <c r="H223" s="4"/>
-    </row>
-    <row r="224" spans="2:8">
+    <row r="223" spans="1:8">
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+    </row>
+    <row r="224" spans="1:8">
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
     </row>
@@ -11212,30 +11280,30 @@
       <c r="G230" s="4"/>
       <c r="H230" s="4"/>
     </row>
-    <row r="233" spans="7:8">
-      <c r="G233" s="3"/>
-      <c r="H233" s="3"/>
+    <row r="231" spans="7:8">
+      <c r="G231" s="4"/>
+      <c r="H231" s="4"/>
+    </row>
+    <row r="232" spans="7:8">
+      <c r="G232" s="4"/>
+      <c r="H232" s="4"/>
     </row>
     <row r="235" spans="7:8">
-      <c r="G235" s="4"/>
-      <c r="H235" s="4"/>
-    </row>
-    <row r="236" spans="7:8">
-      <c r="G236" s="4"/>
-      <c r="H236" s="4"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
     </row>
     <row r="237" spans="7:8">
       <c r="G237" s="4"/>
       <c r="H237" s="4"/>
     </row>
+    <row r="238" spans="7:8">
+      <c r="G238" s="4"/>
+      <c r="H238" s="4"/>
+    </row>
     <row r="239" spans="7:8">
       <c r="G239" s="4"/>
       <c r="H239" s="4"/>
     </row>
-    <row r="240" spans="7:8">
-      <c r="G240" s="4"/>
-      <c r="H240" s="4"/>
-    </row>
     <row r="241" spans="7:8">
       <c r="G241" s="4"/>
       <c r="H241" s="4"/>
@@ -11244,17 +11312,25 @@
       <c r="G242" s="4"/>
       <c r="H242" s="4"/>
     </row>
+    <row r="243" spans="7:8">
+      <c r="G243" s="4"/>
+      <c r="H243" s="4"/>
+    </row>
     <row r="244" spans="7:8">
       <c r="G244" s="4"/>
       <c r="H244" s="4"/>
     </row>
-    <row r="245" spans="7:8">
-      <c r="G245" s="4"/>
-      <c r="H245" s="4"/>
-    </row>
     <row r="246" spans="7:8">
       <c r="G246" s="4"/>
       <c r="H246" s="4"/>
+    </row>
+    <row r="247" spans="7:8">
+      <c r="G247" s="4"/>
+      <c r="H247" s="4"/>
+    </row>
+    <row r="248" spans="7:8">
+      <c r="G248" s="4"/>
+      <c r="H248" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
drc; Edited r0ER11_calc.m to record NaN for r0ER11 in the cases of large fcor and large r_rad, for which the guessed value for rmax becomes so large that the assumption that M_max ~ r_max*V_max breaks down
</commit_message>
<xml_diff>
--- a/Master_simulation_list.xlsx
+++ b/Master_simulation_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="412">
   <si>
     <t>RCE sim</t>
   </si>
@@ -985,9 +985,6 @@
     <t>"0.5" instead of ".5" 0-200</t>
   </si>
   <si>
-    <t>HOPRU6N</t>
-  </si>
-  <si>
     <t>blow up</t>
   </si>
   <si>
@@ -1246,16 +1243,19 @@
     <t>CTRLv0qro80000qrhSATqdz5000_nx3072_fdiv4_lh6000</t>
   </si>
   <si>
+    <t>HOPRU2N</t>
+  </si>
+  <si>
     <t xml:space="preserve">RCE_nx48_SST287.50K_Tthresh200K_usfc3 </t>
   </si>
   <si>
     <t xml:space="preserve">RCE_nx48_SST292.50K_Tthresh200K_usfc3 </t>
   </si>
   <si>
-    <t>RU1N</t>
-  </si>
-  <si>
-    <t>RU2N</t>
+    <t>CTRLv0qrhSATqdz5000_nx3072_SST287.50K</t>
+  </si>
+  <si>
+    <t>CTRLv0qrhSATqdz5000_nx3072_SST292.50K</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1339,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2605">
+  <cellStyleXfs count="2621">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3981,7 +3997,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2605">
+  <cellStyles count="2621">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5284,6 +5300,14 @@
     <cellStyle name="Followed Hyperlink" xfId="2600" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2602" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2620" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6586,6 +6610,14 @@
     <cellStyle name="Hyperlink" xfId="2599" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2601" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2619" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6917,7 +6949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
@@ -8527,7 +8559,13 @@
         <v>408</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>411</v>
+        <v>151</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>407</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="5"/>
@@ -8571,9 +8609,14 @@
         <v>409</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="G86" s="6"/>
+        <v>151</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="I86" s="2"/>
       <c r="J86" s="5"/>
       <c r="K86" s="2"/>
@@ -10235,36 +10278,36 @@
         <v>146</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G160" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K160" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L160" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="161" spans="2:12">
       <c r="F161" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G161" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H161" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K161" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L161" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="2:12">
@@ -10281,27 +10324,27 @@
         <v>146</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G162" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I162" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="163" spans="2:12">
       <c r="F163" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G163" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H163" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="164" spans="2:12">
@@ -10322,30 +10365,30 @@
         <v>146</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G165" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H165" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="2:12">
       <c r="F166" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G166" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K166" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="167" spans="2:12">
@@ -10362,24 +10405,24 @@
         <v>146</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G167" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H167" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="2:12">
       <c r="F168" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G168" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="169" spans="2:12">
@@ -10400,30 +10443,30 @@
         <v>146</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G170" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="171" spans="2:12">
       <c r="F171" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G171" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H171" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K171" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L171" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="172" spans="2:12">
@@ -10440,24 +10483,24 @@
         <v>146</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G172" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="173" spans="2:12">
       <c r="F173" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G173" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H173" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L173" s="3"/>
     </row>
@@ -10479,24 +10522,24 @@
         <v>146</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G175" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H175" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="176" spans="2:12">
       <c r="F176" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G176" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="177" spans="2:12">
@@ -10513,24 +10556,24 @@
         <v>146</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G177" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H177" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="178" spans="2:12">
       <c r="F178" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G178" s="6" t="s">
         <v>151</v>
       </c>
       <c r="H178" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="179" spans="2:12">
@@ -10551,25 +10594,25 @@
         <v>146</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G180" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H180" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L180" s="3"/>
     </row>
     <row r="181" spans="2:12" ht="18">
       <c r="F181" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G181" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L181" s="11"/>
     </row>
@@ -10587,24 +10630,24 @@
         <v>146</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G182" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H182" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="183" spans="2:12">
       <c r="F183" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G183" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="184" spans="2:12">
@@ -10625,30 +10668,30 @@
         <v>146</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G185" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H185" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K185" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="186" spans="2:12">
       <c r="F186" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G186" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="187" spans="2:12">
@@ -10665,30 +10708,30 @@
         <v>146</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G187" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K187" s="5" t="s">
-        <v>321</v>
+        <v>151</v>
       </c>
       <c r="L187" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="188" spans="2:12">
       <c r="F188" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G188" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H188" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="189" spans="2:12">
@@ -10710,30 +10753,30 @@
         <v>146</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G190" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K190" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L190" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="191" spans="2:12">
       <c r="F191" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G191" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H191" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="192" spans="2:12">
@@ -10750,30 +10793,30 @@
         <v>146</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G192" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H192" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K192" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L192" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="193" spans="1:16">
       <c r="F193" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G193" s="6" t="s">
         <v>151</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="194" spans="1:16">
@@ -10794,39 +10837,39 @@
         <v>146</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G195" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I195" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K195" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="L195" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="196" spans="1:16">
       <c r="F196" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G196" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K196" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L196" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="197" spans="1:16">
@@ -10843,28 +10886,28 @@
         <v>146</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G197" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H197" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I197" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K197" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L197" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M197" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O197" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P197" s="4" t="s">
         <v>67</v>
@@ -10872,22 +10915,22 @@
     </row>
     <row r="198" spans="1:16">
       <c r="F198" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G198" s="9" t="s">
         <v>151</v>
       </c>
       <c r="H198" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K198" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L198" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M198" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="199" spans="1:16">
@@ -10895,10 +10938,10 @@
       <c r="G199" s="3"/>
       <c r="H199" s="3"/>
       <c r="O199" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P199" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="200" spans="1:16">
@@ -10915,36 +10958,36 @@
         <v>146</v>
       </c>
       <c r="F200" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G200" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K200" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L200" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="201" spans="1:16">
       <c r="F201" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G201" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H201" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K201" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L201" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="202" spans="1:16">
@@ -10961,30 +11004,30 @@
         <v>146</v>
       </c>
       <c r="F202" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G202" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H202" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K202" s="5" t="s">
         <v>151</v>
       </c>
       <c r="L202" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="203" spans="1:16">
       <c r="F203" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G203" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H203" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="204" spans="1:16">
@@ -11020,15 +11063,15 @@
     </row>
     <row r="207" spans="1:16">
       <c r="A207" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F207" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="208" spans="1:16">
       <c r="A208" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B208" t="s">
         <v>117</v>
@@ -11046,12 +11089,12 @@
         <v>54</v>
       </c>
       <c r="G208" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="209" spans="1:8">
       <c r="A209" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>128</v>
@@ -11066,18 +11109,18 @@
         <v>146</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G209" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H209" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="210" spans="1:8">
       <c r="A210" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B210" t="s">
         <v>117</v>
@@ -11092,13 +11135,13 @@
         <v>146</v>
       </c>
       <c r="F210" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G210" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H210" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -11115,13 +11158,13 @@
         <v>146</v>
       </c>
       <c r="F211" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G211" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H211" s="4" t="s">
         <v>400</v>
-      </c>
-      <c r="G211" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H211" s="4" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -11143,13 +11186,13 @@
         <v>146</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G213" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H213" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -11166,13 +11209,13 @@
         <v>146</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G214" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H214" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -11189,13 +11232,13 @@
         <v>146</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G215" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H215" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -11212,13 +11255,13 @@
         <v>146</v>
       </c>
       <c r="F216" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G216" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H216" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="217" spans="1:8">

</xml_diff>

<commit_message>
drc; Updated TC_super.m files and radprof_evol.m and rz_plot.m to accomodate dry simulations (which do not include moisture variables).
</commit_message>
<xml_diff>
--- a/Master_simulation_list.xlsx
+++ b/Master_simulation_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="427">
   <si>
     <t>RCE sim</t>
   </si>
@@ -1291,12 +1291,6 @@
     <t>CTRLv0qrhSATqdz5000_nx3072_Tthresh150K_fdiv2_lh187.5_tsadapt</t>
   </si>
   <si>
-    <t>RU1N</t>
-  </si>
-  <si>
-    <t>RU2N</t>
-  </si>
-  <si>
     <t>CTRLv0qrhSATqdz5000_nx3072_DRYdrc</t>
   </si>
   <si>
@@ -1304,6 +1298,9 @@
   </si>
   <si>
     <t>RCE_nx48_SST300.00K_Tthresh250K_usfc3_DRY</t>
+  </si>
+  <si>
+    <t>done150, running to 300</t>
   </si>
 </sst>
 </file>
@@ -1387,8 +1384,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2751">
+  <cellStyleXfs count="2765">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4175,7 +4186,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2751">
+  <cellStyles count="2765">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5551,6 +5562,13 @@
     <cellStyle name="Followed Hyperlink" xfId="2746" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2748" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2764" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6926,6 +6944,13 @@
     <cellStyle name="Hyperlink" xfId="2745" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2747" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2763" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7258,7 +7283,7 @@
   <dimension ref="A1:V252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A224" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C236" sqref="C236"/>
+      <selection activeCell="H234" sqref="H234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11746,17 +11771,21 @@
         <v>146</v>
       </c>
       <c r="F233" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="G233" s="4"/>
-      <c r="H233" s="4"/>
+        <v>423</v>
+      </c>
+      <c r="G233" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="H233" s="4" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="234" spans="1:8">
       <c r="B234" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>423</v>
+        <v>150</v>
       </c>
       <c r="D234">
         <v>40</v>
@@ -11766,10 +11795,10 @@
     </row>
     <row r="235" spans="1:8">
       <c r="B235" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>424</v>
+        <v>150</v>
       </c>
       <c r="D235">
         <v>32</v>

</xml_diff>

<commit_message>
drc; Fixed bug in TC_stats.m for 'numfiles' which counted files named 'cm1out_0*.nc'; now it counts files named 'cm1out_*.nc', and thus will work for simulations with >=1000 output files.
</commit_message>
<xml_diff>
--- a/Master_simulation_list.xlsx
+++ b/Master_simulation_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="434">
   <si>
     <t>RCE sim</t>
   </si>
@@ -1291,6 +1291,12 @@
     <t>CTRLv0qrhSATqdz5000_nx3072_Tthresh150K_fdiv2_lh187.5_tsadapt</t>
   </si>
   <si>
+    <t>RU1N</t>
+  </si>
+  <si>
+    <t>RU2N</t>
+  </si>
+  <si>
     <t>CTRLv0qrhSATqdz5000_nx3072_DRYdrc</t>
   </si>
   <si>
@@ -1301,6 +1307,21 @@
   </si>
   <si>
     <t>done150, running to 300</t>
+  </si>
+  <si>
+    <t>RCE_nx48_SST300.00K_Tthresh225K_usfc3_DRY</t>
+  </si>
+  <si>
+    <t>RCE_nx48_SST300.00K_Tthresh175K_usfc3_DRY</t>
+  </si>
+  <si>
+    <t>CTRLv0qrhSATqdz5000_nx3072_tap1hr</t>
+  </si>
+  <si>
+    <t>HOPRU2N</t>
+  </si>
+  <si>
+    <t>hourly output</t>
   </si>
 </sst>
 </file>
@@ -1384,8 +1405,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2765">
+  <cellStyleXfs count="2789">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4186,7 +4231,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2765">
+  <cellStyles count="2789">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5569,6 +5614,18 @@
     <cellStyle name="Followed Hyperlink" xfId="2760" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2762" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2788" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6951,6 +7008,18 @@
     <cellStyle name="Hyperlink" xfId="2759" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2761" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2787" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7282,8 +7351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H234" sqref="H234"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H241" sqref="H241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11759,60 +11828,95 @@
     </row>
     <row r="233" spans="1:8">
       <c r="B233" t="s">
-        <v>420</v>
-      </c>
-      <c r="C233" s="7">
-        <v>10</v>
+        <v>426</v>
+      </c>
+      <c r="C233" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="D233">
         <v>40</v>
-      </c>
-      <c r="E233" t="s">
-        <v>146</v>
-      </c>
-      <c r="F233" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="G233" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="H233" s="4" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="234" spans="1:8">
       <c r="B234" t="s">
+        <v>430</v>
+      </c>
+      <c r="C234" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="C234" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D234">
-        <v>40</v>
       </c>
       <c r="G234" s="4"/>
       <c r="H234" s="4"/>
     </row>
     <row r="235" spans="1:8">
       <c r="B235" t="s">
+        <v>420</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D235">
+        <v>40</v>
+      </c>
+      <c r="E235" t="s">
+        <v>146</v>
+      </c>
+      <c r="F235" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C235" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D235">
-        <v>32</v>
-      </c>
-      <c r="G235" s="4"/>
-      <c r="H235" s="4"/>
+      <c r="G235" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="H235" s="4" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="236" spans="1:8">
+      <c r="B236" t="s">
+        <v>429</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>423</v>
+      </c>
       <c r="G236" s="4"/>
       <c r="H236" s="4"/>
+    </row>
+    <row r="237" spans="1:8">
+      <c r="B237" t="s">
+        <v>427</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D237">
+        <v>32</v>
+      </c>
     </row>
     <row r="239" spans="1:8">
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
+    </row>
+    <row r="240" spans="1:8">
+      <c r="B240" t="s">
+        <v>135</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D240">
+        <v>40</v>
+      </c>
+      <c r="E240" t="s">
+        <v>146</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G240" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="241" spans="7:8">
       <c r="G241" s="4"/>

</xml_diff>